<commit_message>
[bug] modify charger plug-in detect and how to control chg mos
</commit_message>
<xml_diff>
--- a/ lev-gen2-stm8s005k6/src/New_LEVD1_measement.xlsx
+++ b/ lev-gen2-stm8s005k6/src/New_LEVD1_measement.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="19395" windowHeight="8055" activeTab="4"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="19395" windowHeight="8055" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Current校正用" sheetId="8" r:id="rId1"/>
@@ -1916,66 +1916,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="33" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="36" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="36" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
@@ -1993,6 +1933,66 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="33" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="36" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="36" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2023,7 +2023,7 @@
           <c:x val="7.2207084468664848E-2"/>
           <c:y val="6.5645584362161905E-2"/>
           <c:w val="0.60354223433242504"/>
-          <c:h val="0.8161934322362151"/>
+          <c:h val="0.81619343223621521"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -2298,11 +2298,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="84140800"/>
-        <c:axId val="84142720"/>
+        <c:axId val="76616832"/>
+        <c:axId val="76618752"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="84140800"/>
+        <c:axId val="76616832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2335,12 +2335,12 @@
             <a:endParaRPr lang="zh-TW"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="84142720"/>
+        <c:crossAx val="76618752"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="84142720"/>
+        <c:axId val="76618752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2383,7 +2383,7 @@
             <a:endParaRPr lang="zh-TW"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="84140800"/>
+        <c:crossAx val="76616832"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2405,7 +2405,7 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.72070844686648783"/>
+          <c:x val="0.72070844686648794"/>
           <c:y val="0.41794355377243081"/>
           <c:w val="0.26839237057220738"/>
           <c:h val="0.11159749341567524"/>
@@ -2473,7 +2473,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter alignWithMargins="0"/>
-    <c:pageMargins b="1" l="0.75000000000000222" r="0.75000000000000222" t="1" header="0.5" footer="0.5"/>
+    <c:pageMargins b="1" l="0.75000000000000233" r="0.75000000000000233" t="1" header="0.5" footer="0.5"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2491,8 +2491,8 @@
           <c:yMode val="edge"/>
           <c:x val="0.10252109253634827"/>
           <c:y val="7.6923269539436984E-2"/>
-          <c:w val="0.50084074714478544"/>
-          <c:h val="0.78461734930225313"/>
+          <c:w val="0.50084074714478555"/>
+          <c:h val="0.78461734930225291"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -2839,11 +2839,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="84769024"/>
-        <c:axId val="84783488"/>
+        <c:axId val="68864640"/>
+        <c:axId val="76808960"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="84769024"/>
+        <c:axId val="68864640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2876,12 +2876,12 @@
             <a:endParaRPr lang="zh-TW"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="84783488"/>
+        <c:crossAx val="76808960"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="84783488"/>
+        <c:axId val="76808960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2924,7 +2924,7 @@
             <a:endParaRPr lang="zh-TW"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="84769024"/>
+        <c:crossAx val="68864640"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2946,9 +2946,9 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.6521013754771029"/>
+          <c:x val="0.65210137547710301"/>
           <c:y val="0.40512921957436798"/>
-          <c:w val="0.33445405597923661"/>
+          <c:w val="0.33445405597923672"/>
           <c:h val="0.13076955821704281"/>
         </c:manualLayout>
       </c:layout>
@@ -3014,7 +3014,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter alignWithMargins="0"/>
-    <c:pageMargins b="1" l="0.75000000000000222" r="0.75000000000000222" t="1" header="0.5" footer="0.5"/>
+    <c:pageMargins b="1" l="0.75000000000000233" r="0.75000000000000233" t="1" header="0.5" footer="0.5"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3030,10 +3030,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="7.2902387340947852E-2"/>
+          <c:x val="7.2902387340947866E-2"/>
           <c:y val="8.1301028172182765E-2"/>
           <c:w val="0.79229764355444865"/>
-          <c:h val="0.77235976763573544"/>
+          <c:h val="0.77235976763573555"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -3260,11 +3260,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="85066496"/>
-        <c:axId val="85068032"/>
+        <c:axId val="76919552"/>
+        <c:axId val="76921472"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="85066496"/>
+        <c:axId val="76919552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3297,12 +3297,12 @@
             <a:endParaRPr lang="zh-TW"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="85068032"/>
+        <c:crossAx val="76921472"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="85068032"/>
+        <c:axId val="76921472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3345,7 +3345,7 @@
             <a:endParaRPr lang="zh-TW"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="85066496"/>
+        <c:crossAx val="76919552"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3367,10 +3367,10 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.89408588248332033"/>
-          <c:y val="0.39837503804369517"/>
+          <c:x val="0.89408588248332044"/>
+          <c:y val="0.39837503804369523"/>
           <c:w val="9.4910655217460005E-2"/>
-          <c:h val="0.13821174789271093"/>
+          <c:h val="0.13821174789271096"/>
         </c:manualLayout>
       </c:layout>
       <c:spPr>
@@ -3435,7 +3435,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter alignWithMargins="0"/>
-    <c:pageMargins b="1" l="0.75000000000000222" r="0.75000000000000222" t="1" header="0.5" footer="0.5"/>
+    <c:pageMargins b="1" l="0.75000000000000233" r="0.75000000000000233" t="1" header="0.5" footer="0.5"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -4022,19 +4022,19 @@
       </c>
     </row>
     <row r="8" spans="3:21" ht="17.25" thickTop="1">
-      <c r="C8" s="86" t="s">
+      <c r="C8" s="92" t="s">
         <v>153</v>
       </c>
-      <c r="D8" s="87"/>
+      <c r="D8" s="93"/>
       <c r="E8" s="63">
         <v>2000</v>
       </c>
       <c r="F8" s="12"/>
       <c r="G8" s="13"/>
-      <c r="H8" s="88" t="s">
+      <c r="H8" s="94" t="s">
         <v>138</v>
       </c>
-      <c r="I8" s="88"/>
+      <c r="I8" s="94"/>
       <c r="J8" s="62">
         <v>49</v>
       </c>
@@ -4067,20 +4067,20 @@
       </c>
     </row>
     <row r="9" spans="3:21">
-      <c r="C9" s="84" t="s">
+      <c r="C9" s="90" t="s">
         <v>155</v>
       </c>
-      <c r="D9" s="85"/>
+      <c r="D9" s="91"/>
       <c r="E9" s="64">
         <f>ROUND(E8*E6,0)</f>
         <v>197</v>
       </c>
       <c r="F9" s="64"/>
       <c r="G9" s="15"/>
-      <c r="H9" s="88" t="s">
+      <c r="H9" s="94" t="s">
         <v>152</v>
       </c>
-      <c r="I9" s="88"/>
+      <c r="I9" s="94"/>
       <c r="J9">
         <f>ROUND(J8/E6,0)</f>
         <v>498</v>
@@ -4114,10 +4114,10 @@
       </c>
     </row>
     <row r="10" spans="3:21">
-      <c r="C10" s="84" t="s">
+      <c r="C10" s="90" t="s">
         <v>141</v>
       </c>
-      <c r="D10" s="85"/>
+      <c r="D10" s="91"/>
       <c r="E10" s="65">
         <v>188</v>
       </c>
@@ -4152,10 +4152,10 @@
       </c>
     </row>
     <row r="11" spans="3:21">
-      <c r="C11" s="84" t="s">
+      <c r="C11" s="90" t="s">
         <v>142</v>
       </c>
-      <c r="D11" s="85"/>
+      <c r="D11" s="91"/>
       <c r="E11" s="64">
         <f>E10-E9</f>
         <v>-9</v>
@@ -5134,48 +5134,48 @@
     </row>
     <row r="5" spans="3:10" ht="17.25" thickBot="1"/>
     <row r="6" spans="3:10" ht="17.25" thickTop="1">
-      <c r="C6" s="86" t="s">
+      <c r="C6" s="92" t="s">
         <v>139</v>
       </c>
-      <c r="D6" s="87"/>
+      <c r="D6" s="93"/>
       <c r="E6" s="63">
         <v>36000</v>
       </c>
       <c r="F6" s="12"/>
       <c r="G6" s="13"/>
-      <c r="H6" s="88" t="s">
+      <c r="H6" s="94" t="s">
         <v>138</v>
       </c>
-      <c r="I6" s="88"/>
+      <c r="I6" s="94"/>
       <c r="J6" s="62">
         <v>814</v>
       </c>
     </row>
     <row r="7" spans="3:10">
-      <c r="C7" s="84" t="s">
+      <c r="C7" s="90" t="s">
         <v>155</v>
       </c>
-      <c r="D7" s="85"/>
+      <c r="D7" s="91"/>
       <c r="E7" s="58">
         <f>ROUND(E6*E4,0)</f>
         <v>611</v>
       </c>
       <c r="F7" s="58"/>
       <c r="G7" s="15"/>
-      <c r="H7" s="88" t="s">
+      <c r="H7" s="94" t="s">
         <v>140</v>
       </c>
-      <c r="I7" s="88"/>
+      <c r="I7" s="94"/>
       <c r="J7">
         <f>ROUND(J6/E4,0)</f>
         <v>47990</v>
       </c>
     </row>
     <row r="8" spans="3:10">
-      <c r="C8" s="84" t="s">
+      <c r="C8" s="90" t="s">
         <v>141</v>
       </c>
-      <c r="D8" s="85"/>
+      <c r="D8" s="91"/>
       <c r="E8" s="59">
         <v>620</v>
       </c>
@@ -5183,10 +5183,10 @@
       <c r="G8" s="15"/>
     </row>
     <row r="9" spans="3:10">
-      <c r="C9" s="84" t="s">
+      <c r="C9" s="90" t="s">
         <v>142</v>
       </c>
-      <c r="D9" s="85"/>
+      <c r="D9" s="91"/>
       <c r="E9" s="58">
         <f>E8-E7</f>
         <v>9</v>
@@ -5298,8 +5298,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="C2:P50"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -5370,18 +5370,18 @@
       <c r="F5" s="31"/>
       <c r="G5" s="83"/>
       <c r="H5" s="54"/>
-      <c r="I5" s="89" t="s">
+      <c r="I5" s="102" t="s">
         <v>101</v>
       </c>
-      <c r="J5" s="89"/>
-      <c r="K5" s="93" t="s">
+      <c r="J5" s="102"/>
+      <c r="K5" s="103" t="s">
         <v>105</v>
       </c>
-      <c r="L5" s="93"/>
-      <c r="M5" s="93" t="s">
+      <c r="L5" s="103"/>
+      <c r="M5" s="103" t="s">
         <v>106</v>
       </c>
-      <c r="N5" s="97"/>
+      <c r="N5" s="104"/>
     </row>
     <row r="6" spans="3:16" ht="17.25" thickBot="1">
       <c r="C6" s="41" t="s">
@@ -5399,20 +5399,20 @@
       <c r="H6" s="55" t="s">
         <v>100</v>
       </c>
-      <c r="I6" s="90">
+      <c r="I6" s="105">
         <v>4000</v>
       </c>
-      <c r="J6" s="90"/>
-      <c r="K6" s="94">
+      <c r="J6" s="105"/>
+      <c r="K6" s="106">
         <f>I6*E10+E9</f>
         <v>297.89090909090908</v>
       </c>
-      <c r="L6" s="94"/>
-      <c r="M6" s="94">
+      <c r="L6" s="106"/>
+      <c r="M6" s="106">
         <f>I6/10</f>
         <v>400</v>
       </c>
-      <c r="N6" s="98"/>
+      <c r="N6" s="107"/>
     </row>
     <row r="7" spans="3:16" ht="18" thickTop="1" thickBot="1">
       <c r="C7" s="14" t="s">
@@ -5434,20 +5434,20 @@
       <c r="H7" s="55" t="s">
         <v>102</v>
       </c>
-      <c r="I7" s="91">
+      <c r="I7" s="95">
         <v>8000</v>
       </c>
-      <c r="J7" s="91"/>
-      <c r="K7" s="95">
+      <c r="J7" s="95"/>
+      <c r="K7" s="96">
         <f>I7*E13+E12</f>
         <v>407.11757575757576</v>
       </c>
-      <c r="L7" s="95"/>
-      <c r="M7" s="95">
+      <c r="L7" s="96"/>
+      <c r="M7" s="96">
         <f>I7/10</f>
         <v>800</v>
       </c>
-      <c r="N7" s="99"/>
+      <c r="N7" s="98"/>
     </row>
     <row r="8" spans="3:16">
       <c r="C8" s="42" t="s">
@@ -5462,18 +5462,18 @@
       <c r="F8" s="83"/>
       <c r="G8" s="83"/>
       <c r="H8" s="56"/>
-      <c r="I8" s="92" t="s">
+      <c r="I8" s="99" t="s">
         <v>107</v>
       </c>
-      <c r="J8" s="92"/>
-      <c r="K8" s="96" t="s">
+      <c r="J8" s="99"/>
+      <c r="K8" s="100" t="s">
         <v>105</v>
       </c>
-      <c r="L8" s="96"/>
-      <c r="M8" s="96" t="s">
+      <c r="L8" s="100"/>
+      <c r="M8" s="100" t="s">
         <v>106</v>
       </c>
-      <c r="N8" s="100"/>
+      <c r="N8" s="101"/>
     </row>
     <row r="9" spans="3:16" ht="17.25" thickBot="1">
       <c r="C9" s="51"/>
@@ -5490,20 +5490,20 @@
       <c r="H9" s="57" t="s">
         <v>21</v>
       </c>
-      <c r="I9" s="91">
+      <c r="I9" s="95">
         <v>41.6</v>
       </c>
-      <c r="J9" s="91"/>
-      <c r="K9" s="95">
+      <c r="J9" s="95"/>
+      <c r="K9" s="96">
         <f>I9*1000*E17+E16</f>
         <v>534.55883993307316</v>
       </c>
-      <c r="L9" s="95"/>
-      <c r="M9" s="95">
+      <c r="L9" s="96"/>
+      <c r="M9" s="96">
         <f>I9/10</f>
         <v>4.16</v>
       </c>
-      <c r="N9" s="101"/>
+      <c r="N9" s="97"/>
     </row>
     <row r="10" spans="3:16">
       <c r="C10" s="43" t="s">
@@ -5569,17 +5569,17 @@
         <v>5</v>
       </c>
       <c r="G14" s="15"/>
-      <c r="H14" s="104" t="s">
+      <c r="H14" s="84" t="s">
         <v>244</v>
       </c>
-      <c r="I14" s="104"/>
-      <c r="J14" s="104"/>
-      <c r="K14" s="104"/>
-      <c r="L14" s="104"/>
-      <c r="M14" s="104"/>
-      <c r="N14" s="104"/>
-      <c r="O14" s="104"/>
-      <c r="P14" s="104"/>
+      <c r="I14" s="84"/>
+      <c r="J14" s="84"/>
+      <c r="K14" s="84"/>
+      <c r="L14" s="84"/>
+      <c r="M14" s="84"/>
+      <c r="N14" s="84"/>
+      <c r="O14" s="84"/>
+      <c r="P14" s="84"/>
     </row>
     <row r="15" spans="3:16">
       <c r="C15" s="14"/>
@@ -5608,16 +5608,16 @@
       <c r="G16" s="15"/>
     </row>
     <row r="17" spans="3:7" ht="17.25" thickBot="1">
-      <c r="C17" s="106" t="s">
+      <c r="C17" s="86" t="s">
         <v>243</v>
       </c>
-      <c r="D17" s="107"/>
-      <c r="E17" s="108">
+      <c r="D17" s="87"/>
+      <c r="E17" s="88">
         <f>1/(D6/(E15/(E15+E14)))</f>
         <v>1.2849972113775797E-2</v>
       </c>
-      <c r="F17" s="109"/>
-      <c r="G17" s="105"/>
+      <c r="F17" s="89"/>
+      <c r="G17" s="85"/>
     </row>
     <row r="18" spans="3:7" ht="17.25" thickTop="1"/>
     <row r="24" spans="3:7">
@@ -5757,6 +5757,12 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="I5:J5"/>
+    <mergeCell ref="K5:L5"/>
+    <mergeCell ref="M5:N5"/>
+    <mergeCell ref="I6:J6"/>
+    <mergeCell ref="K6:L6"/>
+    <mergeCell ref="M6:N6"/>
     <mergeCell ref="I9:J9"/>
     <mergeCell ref="K9:L9"/>
     <mergeCell ref="M9:N9"/>
@@ -5766,12 +5772,6 @@
     <mergeCell ref="I8:J8"/>
     <mergeCell ref="K8:L8"/>
     <mergeCell ref="M8:N8"/>
-    <mergeCell ref="I5:J5"/>
-    <mergeCell ref="K5:L5"/>
-    <mergeCell ref="M5:N5"/>
-    <mergeCell ref="I6:J6"/>
-    <mergeCell ref="K6:L6"/>
-    <mergeCell ref="M6:N6"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5855,18 +5855,18 @@
       <c r="F5" s="31"/>
       <c r="G5" s="10"/>
       <c r="H5" s="54"/>
-      <c r="I5" s="89" t="s">
+      <c r="I5" s="102" t="s">
         <v>101</v>
       </c>
-      <c r="J5" s="89"/>
-      <c r="K5" s="93" t="s">
+      <c r="J5" s="102"/>
+      <c r="K5" s="103" t="s">
         <v>105</v>
       </c>
-      <c r="L5" s="93"/>
-      <c r="M5" s="93" t="s">
+      <c r="L5" s="103"/>
+      <c r="M5" s="103" t="s">
         <v>106</v>
       </c>
-      <c r="N5" s="97"/>
+      <c r="N5" s="104"/>
     </row>
     <row r="6" spans="3:14" ht="17.25" thickBot="1">
       <c r="C6" s="41" t="s">
@@ -5884,20 +5884,20 @@
       <c r="H6" s="55" t="s">
         <v>100</v>
       </c>
-      <c r="I6" s="90">
+      <c r="I6" s="105">
         <v>3000</v>
       </c>
-      <c r="J6" s="90"/>
-      <c r="K6" s="94">
+      <c r="J6" s="105"/>
+      <c r="K6" s="106">
         <f>I6*E10+E9</f>
         <v>294.91200000000003</v>
       </c>
-      <c r="L6" s="94"/>
-      <c r="M6" s="94">
+      <c r="L6" s="106"/>
+      <c r="M6" s="106">
         <f>I6/10</f>
         <v>300</v>
       </c>
-      <c r="N6" s="98"/>
+      <c r="N6" s="107"/>
     </row>
     <row r="7" spans="3:14" ht="18" thickTop="1" thickBot="1">
       <c r="C7" s="14" t="s">
@@ -5919,20 +5919,20 @@
       <c r="H7" s="55" t="s">
         <v>102</v>
       </c>
-      <c r="I7" s="91">
+      <c r="I7" s="95">
         <v>3000</v>
       </c>
-      <c r="J7" s="91"/>
-      <c r="K7" s="95">
+      <c r="J7" s="95"/>
+      <c r="K7" s="96">
         <f>I7*E13+E12</f>
         <v>201.52320000000003</v>
       </c>
-      <c r="L7" s="95"/>
-      <c r="M7" s="95">
+      <c r="L7" s="96"/>
+      <c r="M7" s="96">
         <f>I7/10</f>
         <v>300</v>
       </c>
-      <c r="N7" s="99"/>
+      <c r="N7" s="98"/>
     </row>
     <row r="8" spans="3:14">
       <c r="C8" s="42" t="s">
@@ -5947,18 +5947,18 @@
       <c r="F8" s="10"/>
       <c r="G8" s="10"/>
       <c r="H8" s="56"/>
-      <c r="I8" s="92" t="s">
+      <c r="I8" s="99" t="s">
         <v>107</v>
       </c>
-      <c r="J8" s="92"/>
-      <c r="K8" s="96" t="s">
+      <c r="J8" s="99"/>
+      <c r="K8" s="100" t="s">
         <v>105</v>
       </c>
-      <c r="L8" s="96"/>
-      <c r="M8" s="96" t="s">
+      <c r="L8" s="100"/>
+      <c r="M8" s="100" t="s">
         <v>106</v>
       </c>
-      <c r="N8" s="100"/>
+      <c r="N8" s="101"/>
     </row>
     <row r="9" spans="3:14" ht="17.25" thickBot="1">
       <c r="C9" s="51"/>
@@ -5975,20 +5975,20 @@
       <c r="H9" s="57" t="s">
         <v>21</v>
       </c>
-      <c r="I9" s="91">
+      <c r="I9" s="95">
         <v>20</v>
       </c>
-      <c r="J9" s="91"/>
-      <c r="K9" s="95">
+      <c r="J9" s="95"/>
+      <c r="K9" s="96">
         <f>I9/(E14+E15)*E15*1000/D6+E16</f>
         <v>339.23926380368101</v>
       </c>
-      <c r="L9" s="95"/>
-      <c r="M9" s="95">
+      <c r="L9" s="96"/>
+      <c r="M9" s="96">
         <f>I9/10</f>
         <v>2</v>
       </c>
-      <c r="N9" s="101"/>
+      <c r="N9" s="97"/>
     </row>
     <row r="10" spans="3:14">
       <c r="C10" s="43" t="s">
@@ -6222,21 +6222,21 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="I5:J5"/>
+    <mergeCell ref="I6:J6"/>
+    <mergeCell ref="I7:J7"/>
+    <mergeCell ref="I8:J8"/>
+    <mergeCell ref="I9:J9"/>
+    <mergeCell ref="K5:L5"/>
+    <mergeCell ref="K6:L6"/>
+    <mergeCell ref="K7:L7"/>
+    <mergeCell ref="K8:L8"/>
+    <mergeCell ref="K9:L9"/>
     <mergeCell ref="M5:N5"/>
     <mergeCell ref="M6:N6"/>
     <mergeCell ref="M7:N7"/>
     <mergeCell ref="M8:N8"/>
     <mergeCell ref="M9:N9"/>
-    <mergeCell ref="K5:L5"/>
-    <mergeCell ref="K6:L6"/>
-    <mergeCell ref="K7:L7"/>
-    <mergeCell ref="K8:L8"/>
-    <mergeCell ref="K9:L9"/>
-    <mergeCell ref="I5:J5"/>
-    <mergeCell ref="I6:J6"/>
-    <mergeCell ref="I7:J7"/>
-    <mergeCell ref="I8:J8"/>
-    <mergeCell ref="I9:J9"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6248,7 +6248,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+    <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
@@ -12409,7 +12409,7 @@
       <c r="C4" s="77" t="s">
         <v>164</v>
       </c>
-      <c r="D4" s="103" t="s">
+      <c r="D4" s="109" t="s">
         <v>214</v>
       </c>
       <c r="E4" s="69" t="s">
@@ -12427,7 +12427,7 @@
       <c r="C5" s="77" t="s">
         <v>164</v>
       </c>
-      <c r="D5" s="103"/>
+      <c r="D5" s="109"/>
       <c r="E5" s="69" t="s">
         <v>224</v>
       </c>
@@ -12443,7 +12443,7 @@
       <c r="C6" s="77" t="s">
         <v>164</v>
       </c>
-      <c r="D6" s="103"/>
+      <c r="D6" s="109"/>
       <c r="E6" s="69" t="s">
         <v>227</v>
       </c>
@@ -12459,7 +12459,7 @@
       <c r="C7" s="77" t="s">
         <v>164</v>
       </c>
-      <c r="D7" s="103"/>
+      <c r="D7" s="109"/>
       <c r="E7" s="69" t="s">
         <v>219</v>
       </c>
@@ -12484,7 +12484,7 @@
       <c r="C8" s="77" t="s">
         <v>164</v>
       </c>
-      <c r="D8" s="103"/>
+      <c r="D8" s="109"/>
       <c r="E8" s="69" t="s">
         <v>225</v>
       </c>
@@ -12500,7 +12500,7 @@
       <c r="C9" s="77" t="s">
         <v>164</v>
       </c>
-      <c r="D9" s="103"/>
+      <c r="D9" s="109"/>
       <c r="E9" s="69" t="s">
         <v>228</v>
       </c>
@@ -12516,7 +12516,7 @@
       <c r="C10" s="77" t="s">
         <v>164</v>
       </c>
-      <c r="D10" s="103"/>
+      <c r="D10" s="109"/>
       <c r="E10" s="69" t="s">
         <v>229</v>
       </c>
@@ -12532,7 +12532,7 @@
       <c r="C11" s="77" t="s">
         <v>164</v>
       </c>
-      <c r="D11" s="103"/>
+      <c r="D11" s="109"/>
       <c r="G11" s="79"/>
     </row>
     <row r="12" spans="1:10">
@@ -12545,7 +12545,7 @@
       <c r="C12" s="77" t="s">
         <v>164</v>
       </c>
-      <c r="D12" s="103"/>
+      <c r="D12" s="109"/>
       <c r="G12" s="79"/>
     </row>
     <row r="13" spans="1:10">
@@ -12558,7 +12558,7 @@
       <c r="C13" s="77" t="s">
         <v>164</v>
       </c>
-      <c r="D13" s="103"/>
+      <c r="D13" s="109"/>
       <c r="G13" s="79"/>
     </row>
     <row r="14" spans="1:10">
@@ -12571,7 +12571,7 @@
       <c r="C14" s="77" t="s">
         <v>164</v>
       </c>
-      <c r="D14" s="103"/>
+      <c r="D14" s="109"/>
     </row>
     <row r="15" spans="1:10">
       <c r="A15" s="78" t="s">
@@ -12583,7 +12583,7 @@
       <c r="C15" s="77" t="s">
         <v>164</v>
       </c>
-      <c r="D15" s="103"/>
+      <c r="D15" s="109"/>
     </row>
     <row r="16" spans="1:10">
       <c r="A16" s="76" t="s">
@@ -12593,7 +12593,7 @@
         <v>164</v>
       </c>
       <c r="C16" s="75"/>
-      <c r="D16" s="102" t="s">
+      <c r="D16" s="108" t="s">
         <v>201</v>
       </c>
     </row>
@@ -12605,7 +12605,7 @@
         <v>164</v>
       </c>
       <c r="C17" s="75"/>
-      <c r="D17" s="102"/>
+      <c r="D17" s="108"/>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="76" t="s">
@@ -12615,7 +12615,7 @@
         <v>164</v>
       </c>
       <c r="C18" s="75"/>
-      <c r="D18" s="102"/>
+      <c r="D18" s="108"/>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" s="76" t="s">
@@ -12625,7 +12625,7 @@
         <v>164</v>
       </c>
       <c r="C19" s="75"/>
-      <c r="D19" s="102"/>
+      <c r="D19" s="108"/>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" s="72" t="s">

</xml_diff>